<commit_message>
Profil + Christian + Tournois + Contact + BDD
</commit_message>
<xml_diff>
--- a/Vue/excel/APHB.xlsx
+++ b/Vue/excel/APHB.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\laragon\www\Site-Coelembier\Vue\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90D261D-4510-4325-8135-2EF2B52F7E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="7545" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>AMICALE DE PETANQUE DE LA HAIE BERTRAND</t>
   </si>
@@ -74,61 +79,44 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="36"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
+      <i/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -139,164 +127,158 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="9">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="164" fillId="0" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -312,7 +294,13 @@
     <xdr:ext cx="1066800" cy="1323975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPr id="2" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -324,7 +312,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -621,28 +612,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:7" customHeight="1" ht="46.5">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="6" spans="1:7">
+    <row r="3" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -651,29 +642,29 @@
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" customHeight="1" ht="26.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" customHeight="1" ht="18.75">
-      <c r="A8" s="22" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" customHeight="1" ht="18.75">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -684,7 +675,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -693,7 +684,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" customHeight="1" ht="18.75">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
@@ -708,7 +699,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" customHeight="1" ht="18.75">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
@@ -723,7 +714,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -732,7 +723,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -741,7 +732,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" customHeight="1" ht="21">
+    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
@@ -752,7 +743,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -761,85 +752,85 @@
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" customHeight="1" ht="18.75">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="7"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:7" customHeight="1" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" customHeight="1" ht="18.75">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" customHeight="1" ht="18.75">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-    </row>
-    <row r="21" spans="1:7" customHeight="1" ht="18.75">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
-    </row>
-    <row r="22" spans="1:7" customHeight="1" ht="18.75">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="24"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -848,7 +839,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -858,8 +849,8 @@
       <c r="G24" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="9">
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="B20:G21"/>
     <mergeCell ref="C22:D22"/>
@@ -870,17 +861,8 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:F18"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.98425196850394" right="0.70866141732283" top="0.74803149606299" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.98425196850394003" right="0.70866141732282995" top="0.74803149606299002" bottom="0.74803149606299002" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>